<commit_message>
updated working fixed data sheet read
</commit_message>
<xml_diff>
--- a/RestSharpDemo/data/testdata.xlsx
+++ b/RestSharpDemo/data/testdata.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
-  <si>
-    <t>Test Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Ridentifier</t>
   </si>
@@ -141,6 +138,12 @@
   </si>
   <si>
     <t>TestMethod5</t>
+  </si>
+  <si>
+    <t>TestName</t>
+  </si>
+  <si>
+    <t>TestMethod1</t>
   </si>
 </sst>
 </file>
@@ -975,7 +978,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,128 +989,128 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>